<commit_message>
Update loading icon and improve keyword selection UI
- Changed loading spinner from heart to data analysis icon
- Redesigned keyword selection with professional grid layout
- Added interactive cards with hover effects for better UX
</commit_message>
<xml_diff>
--- a/uploads/Analysis_Result.xlsx
+++ b/uploads/Analysis_Result.xlsx
@@ -482,14 +482,14 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>resume_prajwal_lawankar_1.pdf</t>
+          <t>Prajwal_Niraj_Lawankar_BACV.docx</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>61.72000122070312</v>
+        <v>43.45000076293945</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>1</v>
@@ -498,14 +498,14 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>resume_prajwal_lawankar_11.pdf</t>
+          <t>Prajwal_Niraj_Lawankar_2025CV_1.pdf</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>61.72000122070312</v>
+        <v>43.45000076293945</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>1</v>
@@ -514,14 +514,14 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Prajwal_Niraj_Lawankar_BACV.docx</t>
+          <t>Prajwal_Lawankar_STC_CV_2025.pdf</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>61.02999877929688</v>
+        <v>37.34000015258789</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>3</v>
@@ -530,30 +530,30 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Prajwal_Niraj_Lawankar_2025CV_1.pdf</t>
+          <t>Mubashira_Khan_Operations_Admin_CV.docx21.pdf</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>61.02999877929688</v>
+        <v>36.34000015258789</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Prajwal_Lawankar___cV.pdf</t>
+          <t>Prajwal_Lawankar_SC_CV_2025.pdf</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>60.20999908447266</v>
+        <v>36.2400016784668</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>5</v>
@@ -562,14 +562,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Prajwal_Lawankar_STC_CV_2025.pdf</t>
+          <t>Prajwal_Lawankar___cV.pdf</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
       <c r="C7" t="n">
-        <v>59.59999847412109</v>
+        <v>35.86999893188477</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
@@ -578,14 +578,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Prajwal_Lawankar_SC_CV_2025.pdf</t>
+          <t>Prajwal_Niraj_Lawankar_BAE_CV.docx</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
       <c r="C8" t="n">
-        <v>57.7400016784668</v>
+        <v>35.0099983215332</v>
       </c>
       <c r="D8" t="n">
         <v>7</v>
@@ -594,14 +594,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Prajwal_Niraj_Lawankar_BAE_CV.docx</t>
+          <t>resume_prajwal_lawankar_11.pdf</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
       <c r="C9" t="n">
-        <v>52.11000061035156</v>
+        <v>31.54999923706055</v>
       </c>
       <c r="D9" t="n">
         <v>8</v>
@@ -610,30 +610,30 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Shubham_UK_resume_for_reference.docx</t>
+          <t>resume_prajwal_lawankar_1.pdf</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>66.67</v>
+        <v>33.33</v>
       </c>
       <c r="C10" t="n">
-        <v>62.93000030517578</v>
+        <v>31.54999923706055</v>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Prajwal_Niraj_Lawankar_Tatasteel_CV.docx</t>
+          <t>Prajwal_Niraj_Lawankar_CV.docx</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>66.67</v>
+        <v>33.33</v>
       </c>
       <c r="C11" t="n">
-        <v>53.18000030517578</v>
+        <v>30.59000015258789</v>
       </c>
       <c r="D11" t="n">
         <v>10</v>
@@ -642,14 +642,14 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Prajwal_Niraj_Lawankar_FSP_CV.docx</t>
+          <t>Shubham_UK_resume_for_reference.docx</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>66.67</v>
+        <v>33.33</v>
       </c>
       <c r="C12" t="n">
-        <v>52.13000106811523</v>
+        <v>29.43000030517578</v>
       </c>
       <c r="D12" t="n">
         <v>11</v>
@@ -658,14 +658,14 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Prajwal_Niraj_Lawankar_CV.docx</t>
+          <t>Omkar-resume-2024-DE2.pdf</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>66.67</v>
+        <v>33.33</v>
       </c>
       <c r="C13" t="n">
-        <v>49.25</v>
+        <v>28.01000022888184</v>
       </c>
       <c r="D13" t="n">
         <v>12</v>
@@ -674,14 +674,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Omkar-resume-2024-DE2.pdf</t>
+          <t>Phd_Omkar_CV.pdf</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
       <c r="C14" t="n">
-        <v>37.75</v>
+        <v>26.71999931335449</v>
       </c>
       <c r="D14" t="n">
         <v>13</v>
@@ -690,14 +690,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Prajwal_Niraj_Lawankar_UK_CV.pdf</t>
+          <t>Aishwarya_cv_for_reference.pdf</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>66.67</v>
+        <v>33.33</v>
       </c>
       <c r="C15" t="n">
-        <v>46.34999847412109</v>
+        <v>21.21999931335449</v>
       </c>
       <c r="D15" t="n">
         <v>14</v>
@@ -706,14 +706,14 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Winning_CV_Template_-_Extra_Curriculars.docx</t>
+          <t>PrajwalLawankar_GPM_CL.pdf</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>45.63000106811523</v>
+        <v>39</v>
       </c>
       <c r="D16" t="n">
         <v>15</v>
@@ -722,14 +722,14 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Prajwal_Lawankar_UK_CV_Tailored.docx</t>
+          <t>Prajwal_Niraj_Lawankar_FSP_CV.docx</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>43.06000137329102</v>
+        <v>33.81000137329102</v>
       </c>
       <c r="D17" t="n">
         <v>16</v>
@@ -738,14 +738,14 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Prajwal_Niraj_Lawankar_GS_CV.pdf</t>
+          <t>Prajwal_Niraj_Lawankar_UK_CV.pdf</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>55.56</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>52.43999862670898</v>
+        <v>29.3700008392334</v>
       </c>
       <c r="D18" t="n">
         <v>17</v>
@@ -754,14 +754,14 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PrajwalLawankar_GPM_CL.pdf</t>
+          <t>Prajwal_Niraj_Lawankar_GS_CV.pdf</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>55.56</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>51.52999877929688</v>
+        <v>29.28000068664551</v>
       </c>
       <c r="D19" t="n">
         <v>18</v>
@@ -770,14 +770,14 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Prajwal_Niraj_Lawankar_Avaiva_CV.docx</t>
+          <t>Prajwal_Lawankar_UK_CV_Tailored.docx</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>55.56</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>50.33000183105469</v>
+        <v>28.52000045776367</v>
       </c>
       <c r="D20" t="n">
         <v>19</v>
@@ -786,14 +786,14 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Phd_Omkar_CV.pdf</t>
+          <t>Winning_CV_Template_-_Extra_Curriculars.docx</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>37.34999847412109</v>
+        <v>27.32999992370605</v>
       </c>
       <c r="D21" t="n">
         <v>20</v>
@@ -802,14 +802,14 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Mubashira_Khan_Operations_Admin_CV.docx21.pdf</t>
+          <t>Prajwal_Niraj_Lawankar_Avaiva_CV.docx</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>44.44</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>48</v>
+        <v>25.09000015258789</v>
       </c>
       <c r="D22" t="n">
         <v>21</v>
@@ -818,14 +818,14 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Imerys_CV.pdf</t>
+          <t>Prajwal_Niraj_Lawankar_Tatasteel_CV.docx</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>17.21999931335449</v>
+        <v>23.79000091552734</v>
       </c>
       <c r="D23" t="n">
         <v>22</v>
@@ -834,14 +834,14 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Aishwarya_cv_for_reference.pdf</t>
+          <t>Imerys_CV.pdf</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>33.33</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>28.64999961853027</v>
+        <v>11.4399995803833</v>
       </c>
       <c r="D24" t="n">
         <v>23</v>
@@ -854,10 +854,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>44.44</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>11.36999988555908</v>
+        <v>10.69999980926514</v>
       </c>
       <c r="D25" t="n">
         <v>24</v>

</xml_diff>